<commit_message>
maj des raport et add de E2
</commit_message>
<xml_diff>
--- a/Projet visite/historisation.xlsx
+++ b/Projet visite/historisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flofl\OneDrive\Documents\0-BTS SIO\2023-2024\1PROJET\Projet visite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664EB279-039E-45AE-9337-08E2200315D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F95F9CF-E53F-46E9-B953-70C1D7F0071C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{EF7189AE-624A-401B-A184-3DC60504E456}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
   <si>
     <t>Responsable</t>
   </si>
@@ -71,28 +71,211 @@
     <t>E</t>
   </si>
   <si>
-    <t>E: elementaire</t>
-  </si>
-  <si>
-    <t>ca:calculée</t>
-  </si>
-  <si>
-    <t>co:composée</t>
-  </si>
-  <si>
-    <t>a:donée alphabetique</t>
-  </si>
-  <si>
-    <t>n:numerique</t>
-  </si>
-  <si>
-    <t>AN:alphanumeriqe</t>
-  </si>
-  <si>
     <t>Remarque</t>
   </si>
   <si>
     <t>VERSIOINNING</t>
+  </si>
+  <si>
+    <t>Colonne1</t>
+  </si>
+  <si>
+    <t>id_emp</t>
+  </si>
+  <si>
+    <t>identifiant_employe</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>nom_emp</t>
+  </si>
+  <si>
+    <t>nom_employe</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>prenom_emp</t>
+  </si>
+  <si>
+    <t>prenom_employe</t>
+  </si>
+  <si>
+    <t>Prénom</t>
+  </si>
+  <si>
+    <t>tele_emp</t>
+  </si>
+  <si>
+    <t>telephone_employe</t>
+  </si>
+  <si>
+    <t>mail_emp</t>
+  </si>
+  <si>
+    <t>mail_employe</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>mdp_emp</t>
+  </si>
+  <si>
+    <t>mdp_responsable</t>
+  </si>
+  <si>
+    <t>Mot de passe</t>
+  </si>
+  <si>
+    <t>id_responsable</t>
+  </si>
+  <si>
+    <t>identifiant_responsable</t>
+  </si>
+  <si>
+    <t>id_delegue</t>
+  </si>
+  <si>
+    <t>identifiant_delegue</t>
+  </si>
+  <si>
+    <t>id_visiteur</t>
+  </si>
+  <si>
+    <t>identifant_visiteur</t>
+  </si>
+  <si>
+    <t>id_secteur</t>
+  </si>
+  <si>
+    <t>identifiant_secteur</t>
+  </si>
+  <si>
+    <t>nom_secteur</t>
+  </si>
+  <si>
+    <t>id_region</t>
+  </si>
+  <si>
+    <t>identifiant_region</t>
+  </si>
+  <si>
+    <t>id_medoc</t>
+  </si>
+  <si>
+    <t>identifiant_medicament</t>
+  </si>
+  <si>
+    <t>nom_medoc</t>
+  </si>
+  <si>
+    <t>nom_medicament</t>
+  </si>
+  <si>
+    <t>id_categorie</t>
+  </si>
+  <si>
+    <t>identifiant_categorie</t>
+  </si>
+  <si>
+    <t>nom_categorie</t>
+  </si>
+  <si>
+    <t>identifiant_professionnel_de_sante</t>
+  </si>
+  <si>
+    <t>nom_professionnel_de_sante</t>
+  </si>
+  <si>
+    <t>id_pro</t>
+  </si>
+  <si>
+    <t>nom_pro</t>
+  </si>
+  <si>
+    <t>prenom_pro</t>
+  </si>
+  <si>
+    <t>CP_pro</t>
+  </si>
+  <si>
+    <t>adresse_pro</t>
+  </si>
+  <si>
+    <t>adresse</t>
+  </si>
+  <si>
+    <t>ville_pro</t>
+  </si>
+  <si>
+    <t>mail_pro</t>
+  </si>
+  <si>
+    <t>tele_pro</t>
+  </si>
+  <si>
+    <t>_professionnel_de_sante</t>
+  </si>
+  <si>
+    <t>derniere_visite</t>
+  </si>
+  <si>
+    <t>metier_pro</t>
+  </si>
+  <si>
+    <t>prenom_professionnel_de_sante</t>
+  </si>
+  <si>
+    <t>metier_professionnel_de_sante</t>
+  </si>
+  <si>
+    <t>adresse_professionnel_de_sante</t>
+  </si>
+  <si>
+    <t>code_postale_professionnel_de_sante</t>
+  </si>
+  <si>
+    <t>ville_professionnel_de_sante</t>
+  </si>
+  <si>
+    <t>mail_professionnel_de_sante</t>
+  </si>
+  <si>
+    <t>tele_professionnel_de_sante</t>
+  </si>
+  <si>
+    <t>Co</t>
+  </si>
+  <si>
+    <t>rapport</t>
+  </si>
+  <si>
+    <t>nom</t>
+  </si>
+  <si>
+    <t>nom_region</t>
+  </si>
+  <si>
+    <t>Téléphone</t>
+  </si>
+  <si>
+    <t>Métier</t>
+  </si>
+  <si>
+    <t>généré</t>
+  </si>
+  <si>
+    <t>Identifiant</t>
   </si>
 </sst>
 </file>
@@ -280,24 +463,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -451,6 +616,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -465,12 +646,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -665,16 +848,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{310BB7F2-124B-4E87-89CD-6EE5E60117EA}" name="Tableau2" displayName="Tableau2" ref="G3:M15" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
-  <autoFilter ref="G3:M15" xr:uid="{310BB7F2-124B-4E87-89CD-6EE5E60117EA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{310BB7F2-124B-4E87-89CD-6EE5E60117EA}" name="Tableau2" displayName="Tableau2" ref="G3:M31" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="G3:M31" xr:uid="{310BB7F2-124B-4E87-89CD-6EE5E60117EA}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{69D54AEF-687C-47F9-960A-BAFFE260C842}" name="Nom Conceptuel" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{940D07E3-5588-4B5A-8E6C-0B18FCDB4517}" name="Nom Logique" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{5B5B102C-729C-460D-85AD-9E229BB9F54B}" name="Type" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{0801991E-A6F8-4600-999B-CA05B526154F}" name="Nature" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{FAA8BA0F-F025-4F06-BAFB-956F64708B29}" name="Longueur" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{1AACAFA8-AAEC-488F-9D06-687318B437C6}" name="Remarque" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{1D3A65F3-5E1C-438B-89FD-94600A061102}" name="Exemple de valeur" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{69D54AEF-687C-47F9-960A-BAFFE260C842}" name="Nom Conceptuel" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{940D07E3-5588-4B5A-8E6C-0B18FCDB4517}" name="Nom Logique" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{5B5B102C-729C-460D-85AD-9E229BB9F54B}" name="Type" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{0801991E-A6F8-4600-999B-CA05B526154F}" name="Nature" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{FAA8BA0F-F025-4F06-BAFB-956F64708B29}" name="Longueur" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{1AACAFA8-AAEC-488F-9D06-687318B437C6}" name="Remarque" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{1D3A65F3-5E1C-438B-89FD-94600A061102}" name="Exemple de valeur" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -977,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70C73C2-053D-47D8-949D-0AE0F7129166}">
-  <dimension ref="B2:M15"/>
+  <dimension ref="B2:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:M2"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,15 +1172,18 @@
     <col min="3" max="3" width="19.21875" customWidth="1"/>
     <col min="4" max="4" width="27.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.6640625" customWidth="1"/>
     <col min="13" max="13" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
@@ -1032,7 +1218,7 @@
         <v>8</v>
       </c>
       <c r="L3" s="14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="M3" s="12" t="s">
         <v>9</v>
@@ -1043,16 +1229,24 @@
       <c r="C4" s="5"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="I4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="J4" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K4" s="5">
         <v>50</v>
       </c>
-      <c r="L4" s="5"/>
+      <c r="L4" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
@@ -1060,16 +1254,24 @@
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="I5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="5"/>
+      <c r="J5" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="K5" s="5">
-        <v>50</v>
-      </c>
-      <c r="L5" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
@@ -1077,16 +1279,24 @@
       <c r="C6" s="5"/>
       <c r="D6" s="6"/>
       <c r="E6" s="7"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
+      <c r="G6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="I6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="J6" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="K6" s="5">
-        <v>50</v>
-      </c>
-      <c r="L6" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
@@ -1094,16 +1304,24 @@
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
+      <c r="G7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="I7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="5"/>
+      <c r="J7" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K7" s="5">
-        <v>50</v>
-      </c>
-      <c r="L7" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>76</v>
+      </c>
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.3">
@@ -1111,16 +1329,24 @@
       <c r="C8" s="5"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="5"/>
+      <c r="G8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="I8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="5"/>
+      <c r="J8" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K8" s="5">
-        <v>50</v>
-      </c>
-      <c r="L8" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="M8" s="7"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.3">
@@ -1128,16 +1354,24 @@
       <c r="C9" s="5"/>
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
+      <c r="G9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="I9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="5"/>
+      <c r="J9" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="K9" s="5">
-        <v>50</v>
-      </c>
-      <c r="L9" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="M9" s="7"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.3">
@@ -1145,16 +1379,24 @@
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
       <c r="E10" s="7"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
+      <c r="G10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="I10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="5"/>
+      <c r="J10" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K10" s="5">
-        <v>50</v>
-      </c>
-      <c r="L10" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.3">
@@ -1162,16 +1404,24 @@
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
       <c r="E11" s="7"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
+      <c r="G11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="I11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="J11" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="K11" s="5">
-        <v>50</v>
-      </c>
-      <c r="L11" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.3">
@@ -1179,62 +1429,409 @@
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="11"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9"/>
+      <c r="G12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="5"/>
       <c r="I12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="K12" s="5">
+        <v>20</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="5">
+        <v>5</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M13" s="11"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K14" s="5">
+        <v>10</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M14" s="11"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="5">
+        <v>20</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="G16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K16" s="5">
+        <v>20</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17" s="5">
+        <v>10</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M17" s="7"/>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="5">
         <v>50</v>
       </c>
-      <c r="L12" s="9"/>
-      <c r="M12" s="11"/>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="5">
+      <c r="L18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M18" s="7"/>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="5">
+        <v>10</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" s="7"/>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G20" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="9"/>
-      <c r="M13" s="11"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="5">
-        <v>50</v>
-      </c>
-      <c r="L14" s="9"/>
-      <c r="M14" s="11"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="9" t="s">
+      <c r="H20" s="5"/>
+      <c r="I20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="5">
+        <v>20</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M20" s="7"/>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="5">
-        <v>50</v>
-      </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="11"/>
+      <c r="K21" s="5">
+        <v>10</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M21" s="7"/>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="5">
+        <v>20</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M22" s="7"/>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="5">
+        <v>20</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M23" s="7"/>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" s="5">
+        <v>20</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="M24" s="7"/>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G25" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25" s="9">
+        <v>100</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="5">
+        <v>5</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="7"/>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="5">
+        <v>20</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="7"/>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" s="5">
+        <v>30</v>
+      </c>
+      <c r="L28" s="5"/>
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G29" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="5">
+        <v>10</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M29" s="7"/>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G30" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" s="8"/>
+      <c r="I30" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" s="9">
+        <v>30</v>
+      </c>
+      <c r="L30" s="9"/>
+      <c r="M30" s="11"/>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="G31" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="5">
+        <v>20</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M31" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>